<commit_message>
add 6-11 protect Excel
</commit_message>
<xml_diff>
--- a/part2_Use-Python-in-Office/ch06_work-with-excel/6-8_filtering-sorting/test.xlsx
+++ b/part2_Use-Python-in-Office/ch06_work-with-excel/6-8_filtering-sorting/test.xlsx
@@ -36,7 +36,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -47,6 +47,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -80,10 +86,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -403,7 +409,7 @@
     <col min="4" max="4" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>